<commit_message>
Movendo arquivos para a raiz do repositório
</commit_message>
<xml_diff>
--- a/historico_temperatura.xlsx
+++ b/historico_temperatura.xlsx
@@ -393,7 +393,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -472,6 +472,21 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>28/03/2025 17:03:18</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>20.2</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>94%</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>